<commit_message>
devre ayırıcılar ve teste başla-bitir eklendi
</commit_message>
<xml_diff>
--- a/dokumanlar/AKD.xlsx
+++ b/dokumanlar/AKD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PC2FPGA" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="69">
   <si>
     <t>HEADER</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>CRC LOW</t>
+  </si>
+  <si>
+    <t>TESTE BAŞLA KOMUTU  ---&gt; TESTİ DURDUR</t>
+  </si>
+  <si>
+    <t>TESTE BAŞLA KOMUTU CEVAP --&gt; TESTİ DURDUR</t>
   </si>
 </sst>
 </file>
@@ -318,19 +324,19 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:E53"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,597 +664,592 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B5" s="6" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B9" s="1" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="A9" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B13" s="1" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="A13" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B17" s="1" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="A17" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="A20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="A21" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="A24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B25" s="1" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="A28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B29" s="1" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="A29" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="A32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B33" s="6" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="A33" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="A36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B37" s="6" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="A37" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B37" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="6" t="s">
+      <c r="A40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B41" s="6" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="A41" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B41" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="6" t="s">
+      <c r="A44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B45" s="6" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="A45" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B45" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="A48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E48" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B49" s="6" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C49" s="6" t="s">
+      <c r="A49" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B49" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E49" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="6" t="s">
+      <c r="A52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="str">
-        <f>B1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="B53" s="6" t="str">
-        <f>C1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="C53" s="6" t="s">
+      <c r="A53" s="2" t="str">
+        <f>B1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="B53" s="2" t="str">
+        <f>C1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E53" s="2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A47:E47"/>
     <mergeCell ref="A51:E51"/>
@@ -1257,6 +1258,11 @@
     <mergeCell ref="A31:E31"/>
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1266,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E45" sqref="A43:E45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,652 +1293,652 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B5" s="6" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B9" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="A9" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B13" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="A13" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B17" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="A17" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="A20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="A21" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="A24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B25" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="A28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B29" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="A29" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="A32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B33" s="6" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="A33" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="A36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B37" s="6" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="A37" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B37" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="A40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B41" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="A41" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B41" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="A44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B45" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="A45" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B45" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="A48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B49" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="A49" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B49" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="A52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B53" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="A53" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B53" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="5"/>
+      <c r="A56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="str">
-        <f>B1</f>
-        <v>0xCD</v>
-      </c>
-      <c r="B57" s="1" t="str">
-        <f>C1</f>
-        <v>0xAB</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="A57" s="2" t="str">
+        <f>B1</f>
+        <v>0xCD</v>
+      </c>
+      <c r="B57" s="2" t="str">
+        <f>C1</f>
+        <v>0xAB</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
@@ -2050,12 +2056,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A51:E51"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="C56:E56"/>
@@ -2066,6 +2066,12 @@
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>